<commit_message>
Added Functionality to save test results
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stinagami\Documents\Semester 2\CMPG323\Projects\Project 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stinagami\Documents\GitHub\CMPG-323-Project-4---32151314\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1127,7 +1127,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1245,7 +1245,7 @@
         <v>62</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1262,7 +1262,7 @@
         <v>63</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1279,7 +1279,7 @@
         <v>64</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -1296,7 +1296,7 @@
         <v>65</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>

</xml_diff>